<commit_message>
Database design choices 2
These were the database tables I developed after determining a many to many relationship between authors and books, therefore I created a joining table for authors/books.
</commit_message>
<xml_diff>
--- a/Database design choices.xlsx
+++ b/Database design choices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/109785fd0f6a58e9/Desktop/QA Consulting/Projects/Inventory Management System/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{A25EB117-C4C9-4718-813D-9BDE97FB4D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{239EBC07-2E07-498E-9C65-FD1CBB3EDE89}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{A25EB117-C4C9-4718-813D-9BDE97FB4D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{638FEA87-4CA2-4E2C-883F-E5A9AE7C4CDC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{74251761-EFC5-458D-B31D-40BB8CAA2CE5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="72">
   <si>
     <t xml:space="preserve">Customers Table </t>
   </si>
@@ -59,12 +59,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t xml:space="preserve">Products Table </t>
-  </si>
-  <si>
-    <t>PID</t>
-  </si>
-  <si>
     <t>Author Name</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t xml:space="preserve">DATE </t>
   </si>
   <si>
-    <t>VARCHAR(17)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Field Name </t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>Null constraint is used because of GDPR and customers not having to provide personal details. VACHAR(150) is used as addresses always vary in length and are alphanumeric variables</t>
   </si>
   <si>
-    <t>It is a barcode and contains numbers and hyphens. UNIQUE constraint is used as each book has its own unique ISBN value</t>
-  </si>
-  <si>
     <t>This field must be NOT NULL in order for Book Galore to keep track of Book titles. VARCHAR(320) because book titles vary in length and can be up to 320 characters long</t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t>This field must be NOT NULL in order for Book Galore to keep track of book publishers. VARCHAR(32) because publisher names vary in length and this field shouldn’t need more than 32 characters</t>
   </si>
   <si>
-    <t>Orders_Products Table</t>
-  </si>
-  <si>
     <t>OID</t>
   </si>
   <si>
@@ -200,9 +185,6 @@
     <t>DECIMAL (5,2)</t>
   </si>
   <si>
-    <t>DECIMAL (5,2</t>
-  </si>
-  <si>
     <t>Null constraint is used because of GDPR and customers not having to provide personal details. CHAR(10) is used because postcodes are a fixed length in the UK and don’t go over 10 characters</t>
   </si>
   <si>
@@ -236,10 +218,37 @@
     <t>Since this is a junction table, it is just compiling the PRIMARY KEY of another table. This means OID  will be a FOREIGN KEY in this table as its values do not have to be UNIQUE</t>
   </si>
   <si>
-    <t>Since this is a junction table, it is just compiling the PRIMARY KEY of another table. This means PID will be a FOREIGN KEY in this table as its values do not have to be UNIQUE</t>
-  </si>
-  <si>
     <t>This field must be NOT NULL in order for Book Galore to keep track of bookprices. DECIMAL(5,2) is used to maintain regular format of pricing and purchases can contain 3-digits before the decimal e.g £235.00</t>
+  </si>
+  <si>
+    <t>CHAR(17)</t>
+  </si>
+  <si>
+    <t>UNIQUE constraint is used as each book has its own unique ISBN barcode. CHAR(17) is used because ISBN barcodes have a fixed length of 17 characters, containing numbers and hyphens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Books Table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors Table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AID </t>
+  </si>
+  <si>
+    <t>BID</t>
+  </si>
+  <si>
+    <t>Orders_Books Table</t>
+  </si>
+  <si>
+    <t>Since this is a junction table, it is just compiling the PRIMARY KEY of another table. This means BID will be a FOREIGN KEY in this table as its values do not have to be UNIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors_Books Table </t>
+  </si>
+  <si>
+    <t>Not Null constraint is used because of GDPR and customers not having to provide personal details. Also VACHAR(32) is used as first names always vary in length and first names rarley contain more than 32 characters</t>
   </si>
 </sst>
 </file>
@@ -271,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,8 +311,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3579E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -363,12 +390,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -407,21 +447,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -430,8 +455,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -440,6 +499,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF3579E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -748,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150195B1-47F3-4CC0-90E5-683671A4E85B}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,23 +834,23 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="12"/>
       <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -809,96 +873,96 @@
       <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="24"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="23"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
+      <c r="B6" s="21"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="K6" s="23"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
@@ -908,7 +972,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="K7" s="23"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
@@ -918,342 +982,599 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="8"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="E41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="20"/>
+    </row>
+    <row r="42" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="25"/>
-    </row>
-    <row r="26" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-    </row>
-    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-    </row>
-    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="F42" s="20"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="C44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="22"/>
+    </row>
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22"/>
+    </row>
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A28:A34"/>
+  <mergeCells count="7">
+    <mergeCell ref="A44:A50"/>
     <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B38:E38"/>
     <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>